<commit_message>
Shifting the contents of ShoutOption into functions for portability
</commit_message>
<xml_diff>
--- a/options.xlsx
+++ b/options.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\Github\ShoutOption\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\ShoutOption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{431EC0C2-6E1B-49AE-98C7-F0E9182451F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94B01E8-41A4-4925-98C2-DE2784410BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3083" yWindow="2430" windowWidth="11970" windowHeight="10650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -28,15 +31,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>call</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>strike</t>
   </si>
   <si>
-    <t>put</t>
+    <t>Dec 2020 call</t>
+  </si>
+  <si>
+    <t>Dec 2020 put</t>
+  </si>
+  <si>
+    <t>Jun 2020 call</t>
+  </si>
+  <si>
+    <t>Jun 2020 put</t>
   </si>
 </sst>
 </file>
@@ -46,8 +55,10 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -106,7 +118,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -118,7 +130,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -165,23 +177,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -217,23 +212,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -386,139 +364,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>307500</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>187.4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>148.80000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D2" s="1">
+        <v>165.1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>127.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>308000</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>184.2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>150.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D3" s="1">
+        <v>161.69999999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>128.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>309000</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>178</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>154.30000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D4" s="1">
+        <v>154.9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>131.80000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>310000</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>171.9</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>158.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D5" s="1">
+        <v>148.30000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>135.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>311000</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>166</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>162</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D6" s="1">
+        <v>141.80000000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>138.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>312000</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>160.1</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>166</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D7" s="1">
+        <v>135.4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>312500</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>157.19999999999999</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>168.1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D8" s="1">
+        <v>132.19999999999999</v>
+      </c>
+      <c r="E8" s="1">
+        <v>143.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>313000</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>154.4</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>170.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D9" s="1">
+        <v>129.1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>145.69999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>314000</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>148.80000000000001</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>174.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D10" s="1">
+        <v>122.9</v>
+      </c>
+      <c r="E10" s="1">
+        <v>149.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>315000</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>143.30000000000001</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>178.9</v>
       </c>
+      <c r="D11" s="1">
+        <v>116.9</v>
+      </c>
+      <c r="E11" s="1">
+        <v>153.4</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69124999999999992" right="0.69124999999999992" top="0.74062499999999998" bottom="0.74062499999999998" header="0.29624999999999996" footer="0.29624999999999996"/>
-  <pageSetup paperSize="9" orientation="portrait" copies="0"/>
-  <headerFooter alignWithMargins="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>